<commit_message>
Small fixes to species info (most notably SPAMA to SPAM2)
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/01b_edited6_location-independent-manual-fix.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/01b_edited6_location-independent-manual-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E85D3E-707B-466A-866F-2763D5377A5F}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7AA000D-C579-45B8-9AA1-CB0FFEC88E92}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="1620" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
   <authors>
     <author>tc={BFC3FD45-334D-46E0-9559-012C02335121}</author>
     <author>tc={9C0BAC8A-A827-4EAA-B847-3F7C2899E2A4}</author>
+    <author>tc={9170C499-DD8A-4163-96C6-10F0781B22AB}</author>
     <author>tc={E625EF3B-7C6F-4C78-8D95-22D791DCE7BE}</author>
   </authors>
   <commentList>
@@ -43,7 +44,15 @@
     This is the official USDA Plants code</t>
       </text>
     </comment>
-    <comment ref="B145" authorId="2" shapeId="0" xr:uid="{E625EF3B-7C6F-4C78-8D95-22D791DCE7BE}">
+    <comment ref="B137" authorId="2" shapeId="0" xr:uid="{9170C499-DD8A-4163-96C6-10F0781B22AB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Change so it matches codes in seed mix</t>
+      </text>
+    </comment>
+    <comment ref="B145" authorId="3" shapeId="0" xr:uid="{E625EF3B-7C6F-4C78-8D95-22D791DCE7BE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="304">
   <si>
     <t>CodeOriginal</t>
   </si>
@@ -965,13 +974,16 @@
   </si>
   <si>
     <t>Eragrostis curvula or lehmanniana</t>
+  </si>
+  <si>
+    <t>SPAM2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1117,6 +1129,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1607,6 +1625,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Lia Ossanna" id="{B6FF104B-9E4A-4529-B4A6-6B992DB24262}" userId="S::lossanna@nmsu.edu::46d24f92-a3d9-425c-98e5-f4d1ec18a5c1" providerId="AD"/>
   <person displayName="Ossanna, Lia Qin Ryan - (lossanna)" id="{F2C253AE-3829-426F-8607-10F478AAC97A}" userId="S::lossanna@arizona.edu::4ef914cd-790d-460d-a4af-cca4fc5cf0d2" providerId="AD"/>
 </personList>
 </file>
@@ -1914,6 +1933,9 @@
   <threadedComment ref="B72" dT="2023-09-11T22:15:59.13" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{9C0BAC8A-A827-4EAA-B847-3F7C2899E2A4}">
     <text>This is the official USDA Plants code</text>
   </threadedComment>
+  <threadedComment ref="B137" dT="2025-10-10T17:46:05.22" personId="{B6FF104B-9E4A-4529-B4A6-6B992DB24262}" id="{9170C499-DD8A-4163-96C6-10F0781B22AB}">
+    <text>Change so it matches codes in seed mix</text>
+  </threadedComment>
   <threadedComment ref="B145" dT="2023-09-11T22:17:46.96" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{E625EF3B-7C6F-4C78-8D95-22D791DCE7BE}">
     <text>This is the official USDA Plants code</text>
   </threadedComment>
@@ -1925,8 +1947,8 @@
   <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G136" sqref="G136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4664,8 +4686,8 @@
       <c r="A137" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>269</v>
+      <c r="B137" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>270</v>

</xml_diff>